<commit_message>
deleted old styling and made new one, matching colors and theme, added responsivity to all iPhones available.
</commit_message>
<xml_diff>
--- a/designs/ios pizel sizes.xlsx
+++ b/designs/ios pizel sizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khaht\Desktop\Company-X\designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31807FB2-8D92-4D61-9D1A-EAE19DF8ED03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C61816-D33F-4672-A237-146BF2819733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F990DCC-59DA-4D7C-9F9F-AD37ECA22E05}"/>
+    <workbookView xWindow="-24855" yWindow="1890" windowWidth="16995" windowHeight="11385" xr2:uid="{3F990DCC-59DA-4D7C-9F9F-AD37ECA22E05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,13 +68,13 @@
     <t>iPhone 12 Pro, iPhone 12, iPhone 13, iPhone 14</t>
   </si>
   <si>
-    <t>iPhone 12 Pro Max, iPhone 13 Pro Max, iPhone 14 Plus,</t>
-  </si>
-  <si>
     <t>iPhone 14 Pro,  iPhone 15,  iPhone 15 Pro</t>
   </si>
   <si>
     <t>iPhone 14 Pro Max, iPhone 15 Plus, iPhone 15 Pro Max</t>
+  </si>
+  <si>
+    <t>iPhone 12 Pro Max, iPhone 13 Pro Max, iPhone 14 Plus</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D17">
         <v>428</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <v>393</v>
@@ -557,7 +557,7 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21">
         <v>430</v>
@@ -568,5 +568,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I did mediaquaries from scracth again had some bug. Works on all iPhones.
</commit_message>
<xml_diff>
--- a/designs/ios pizel sizes.xlsx
+++ b/designs/ios pizel sizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khaht\Desktop\Company-X\designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C61816-D33F-4672-A237-146BF2819733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103583C6-E652-414D-9E84-CB4BEA01E4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24855" yWindow="1890" windowWidth="16995" windowHeight="11385" xr2:uid="{3F990DCC-59DA-4D7C-9F9F-AD37ECA22E05}"/>
+    <workbookView xWindow="1260" yWindow="1965" windowWidth="16995" windowHeight="11385" xr2:uid="{3F990DCC-59DA-4D7C-9F9F-AD37ECA22E05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>